<commit_message>
2015.2.2 alert when complete
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -30,1327 +30,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BioPep00050</t>
-  </si>
-  <si>
-    <t>Q9YGH4</t>
-  </si>
-  <si>
-    <t>BioPep00051</t>
-  </si>
-  <si>
-    <t>P01170</t>
-  </si>
-  <si>
-    <t>BioPep00052</t>
-  </si>
-  <si>
-    <t>P09876</t>
-  </si>
-  <si>
-    <t>BioPep00053</t>
-  </si>
-  <si>
-    <t>P21780</t>
-  </si>
-  <si>
-    <t>BioPep00054</t>
-  </si>
-  <si>
-    <t>P81029</t>
-  </si>
-  <si>
-    <t>BioPep00055</t>
-  </si>
-  <si>
-    <t>Q91194</t>
-  </si>
-  <si>
-    <t>BioPep00056</t>
-  </si>
-  <si>
-    <t>BioPep00057</t>
-  </si>
-  <si>
-    <t>Q0VTT8</t>
-  </si>
-  <si>
-    <t>BioPep00058</t>
-  </si>
-  <si>
-    <t>P84897</t>
-  </si>
-  <si>
-    <t>BioPep00059</t>
-  </si>
-  <si>
-    <t>P84935</t>
-  </si>
-  <si>
-    <t>BioPep00060</t>
-  </si>
-  <si>
-    <t>BioPep00061</t>
-  </si>
-  <si>
-    <t>P83057</t>
-  </si>
-  <si>
-    <t>BioPep00062</t>
-  </si>
-  <si>
-    <t>P84673</t>
-  </si>
-  <si>
-    <t>BioPep00063</t>
-  </si>
-  <si>
-    <t>P84894</t>
-  </si>
-  <si>
-    <t>BioPep00064</t>
-  </si>
-  <si>
-    <t>Q0VTU0</t>
-  </si>
-  <si>
-    <t>BioPep00065</t>
-  </si>
-  <si>
-    <t>P84899</t>
-  </si>
-  <si>
-    <t>BioPep00066</t>
-  </si>
-  <si>
-    <t>BioPep00067</t>
-  </si>
-  <si>
-    <t>P84898</t>
-  </si>
-  <si>
-    <t>BioPep00068</t>
-  </si>
-  <si>
-    <t>Q3MQ28</t>
-  </si>
-  <si>
-    <t>BioPep00069</t>
-  </si>
-  <si>
-    <t>P84745</t>
-  </si>
-  <si>
-    <t>BioPep00070</t>
-  </si>
-  <si>
-    <t>P84746</t>
-  </si>
-  <si>
-    <t>BioPep00071</t>
-  </si>
-  <si>
-    <t>P84747</t>
-  </si>
-  <si>
-    <t>BioPep00072</t>
-  </si>
-  <si>
-    <t>P26202</t>
-  </si>
-  <si>
-    <t>BioPep00073</t>
-  </si>
-  <si>
-    <t>P26203</t>
-  </si>
-  <si>
-    <t>BioPep00074</t>
-  </si>
-  <si>
-    <t>P9WJ62</t>
-  </si>
-  <si>
-    <t>BioPep00075</t>
-  </si>
-  <si>
-    <t>P9WJ63</t>
-  </si>
-  <si>
-    <t>BioPep00076</t>
-  </si>
-  <si>
-    <t>P81925</t>
-  </si>
-  <si>
-    <t>BioPep00077</t>
-  </si>
-  <si>
-    <t>P86783</t>
-  </si>
-  <si>
-    <t>BioPep00078</t>
-  </si>
-  <si>
-    <t>BioPep00079</t>
-  </si>
-  <si>
-    <t>Q10722</t>
-  </si>
-  <si>
-    <t>BioPep00080</t>
-  </si>
-  <si>
-    <t>P41965</t>
-  </si>
-  <si>
-    <t>BioPep00081</t>
-  </si>
-  <si>
-    <t>P56686</t>
-  </si>
-  <si>
-    <t>BioPep00082</t>
-  </si>
-  <si>
-    <t>P83328</t>
-  </si>
-  <si>
-    <t>BioPep00083</t>
-  </si>
-  <si>
-    <t>P05516</t>
-  </si>
-  <si>
-    <t>BioPep00084</t>
-  </si>
-  <si>
-    <t>P06575</t>
-  </si>
-  <si>
-    <t>BioPep00085</t>
-  </si>
-  <si>
-    <t>P12963</t>
-  </si>
-  <si>
-    <t>BioPep00086</t>
-  </si>
-  <si>
-    <t>P69053</t>
-  </si>
-  <si>
-    <t>BioPep00087</t>
-  </si>
-  <si>
-    <t>Q5ZT84</t>
-  </si>
-  <si>
-    <t>BioPep00088</t>
-  </si>
-  <si>
-    <t>P15131</t>
-  </si>
-  <si>
-    <t>BioPep00089</t>
-  </si>
-  <si>
-    <t>P56029</t>
-  </si>
-  <si>
-    <t>BioPep00090</t>
-  </si>
-  <si>
-    <t>Q0ZZJ6</t>
-  </si>
-  <si>
-    <t>BioPep00091</t>
-  </si>
-  <si>
-    <t>A0RZC6</t>
-  </si>
-  <si>
-    <t>BioPep00092</t>
-  </si>
-  <si>
-    <t>A5PG36</t>
-  </si>
-  <si>
-    <t>BioPep00093</t>
-  </si>
-  <si>
-    <t>A5PG37</t>
-  </si>
-  <si>
-    <t>BioPep00094</t>
-  </si>
-  <si>
-    <t>A5PG38</t>
-  </si>
-  <si>
-    <t>BioPep00095</t>
-  </si>
-  <si>
-    <t>B2FUW2</t>
-  </si>
-  <si>
-    <t>BioPep00096</t>
-  </si>
-  <si>
-    <t>P41855</t>
-  </si>
-  <si>
-    <t>BioPep00097</t>
-  </si>
-  <si>
-    <t>Q16N80</t>
-  </si>
-  <si>
-    <t>BioPep00098</t>
-  </si>
-  <si>
-    <t>Q7PTL2</t>
-  </si>
-  <si>
-    <t>BioPep00099</t>
-  </si>
-  <si>
-    <t>O44185</t>
-  </si>
-  <si>
-    <t>BioPep00100</t>
-  </si>
-  <si>
-    <t>BioPep00101</t>
-  </si>
-  <si>
-    <t>P10552</t>
-  </si>
-  <si>
-    <t>BioPep00102</t>
-  </si>
-  <si>
-    <t>Q9NDE8</t>
-  </si>
-  <si>
-    <t>BioPep00103</t>
-  </si>
-  <si>
-    <t>P15450</t>
-  </si>
-  <si>
-    <t>BioPep00104</t>
-  </si>
-  <si>
-    <t>P81463</t>
-  </si>
-  <si>
-    <t>BioPep00105</t>
-  </si>
-  <si>
-    <t>P06518</t>
-  </si>
-  <si>
-    <t>BioPep00106</t>
-  </si>
-  <si>
-    <t>P81592</t>
-  </si>
-  <si>
-    <t>BioPep00107</t>
-  </si>
-  <si>
-    <t>BioPep00108</t>
-  </si>
-  <si>
-    <t>BioPep00109</t>
-  </si>
-  <si>
-    <t>BioPep00110</t>
-  </si>
-  <si>
-    <t>BioPep00111</t>
-  </si>
-  <si>
-    <t>Q8I948</t>
-  </si>
-  <si>
-    <t>BioPep00112</t>
-  </si>
-  <si>
-    <t>Q8I6R7</t>
-  </si>
-  <si>
-    <t>BioPep00113</t>
-  </si>
-  <si>
-    <t>P38441</t>
-  </si>
-  <si>
-    <t>BioPep00114</t>
-  </si>
-  <si>
-    <t>P16548</t>
-  </si>
-  <si>
-    <t>BioPep00115</t>
-  </si>
-  <si>
-    <t>P25681</t>
-  </si>
-  <si>
-    <t>BioPep00116</t>
-  </si>
-  <si>
-    <t>P35903</t>
-  </si>
-  <si>
-    <t>BioPep00117</t>
-  </si>
-  <si>
-    <t>P35904</t>
-  </si>
-  <si>
-    <t>BioPep00118</t>
-  </si>
-  <si>
-    <t>P29002</t>
-  </si>
-  <si>
-    <t>BioPep00119</t>
-  </si>
-  <si>
-    <t>P29004</t>
-  </si>
-  <si>
-    <t>BioPep00120</t>
-  </si>
-  <si>
-    <t>P29006</t>
-  </si>
-  <si>
-    <t>BioPep00121</t>
-  </si>
-  <si>
-    <t>BioPep00122</t>
-  </si>
-  <si>
-    <t>BioPep00123</t>
-  </si>
-  <si>
-    <t>BioPep00124</t>
-  </si>
-  <si>
-    <t>P82286</t>
-  </si>
-  <si>
-    <t>BioPep00125</t>
-  </si>
-  <si>
-    <t>BioPep00126</t>
-  </si>
-  <si>
-    <t>BioPep00127</t>
-  </si>
-  <si>
-    <t>BioPep00128</t>
-  </si>
-  <si>
-    <t>P01362</t>
-  </si>
-  <si>
-    <t>BioPep00129</t>
-  </si>
-  <si>
-    <t>P17685</t>
-  </si>
-  <si>
-    <t>BioPep00130</t>
-  </si>
-  <si>
-    <t>P17686</t>
-  </si>
-  <si>
-    <t>BioPep00131</t>
-  </si>
-  <si>
-    <t>BioPep00132</t>
-  </si>
-  <si>
-    <t>BioPep00133</t>
-  </si>
-  <si>
-    <t>BioPep00134</t>
-  </si>
-  <si>
-    <t>BioPep00135</t>
-  </si>
-  <si>
-    <t>BioPep00136</t>
-  </si>
-  <si>
-    <t>BioPep00137</t>
-  </si>
-  <si>
-    <t>BioPep00138</t>
-  </si>
-  <si>
-    <t>P30811</t>
-  </si>
-  <si>
-    <t>BioPep00139</t>
-  </si>
-  <si>
-    <t>P23028</t>
-  </si>
-  <si>
-    <t>BioPep00140</t>
-  </si>
-  <si>
-    <t>P04084</t>
-  </si>
-  <si>
-    <t>BioPep00141</t>
-  </si>
-  <si>
-    <t>A4VBF0</t>
-  </si>
-  <si>
-    <t>BioPep00142</t>
-  </si>
-  <si>
-    <t>Q10754</t>
-  </si>
-  <si>
-    <t>BioPep00143</t>
-  </si>
-  <si>
-    <t>Q8JFG1</t>
-  </si>
-  <si>
-    <t>BioPep00144</t>
-  </si>
-  <si>
-    <t>P01538</t>
-  </si>
-  <si>
-    <t>BioPep00145</t>
-  </si>
-  <si>
-    <t>P01543</t>
-  </si>
-  <si>
-    <t>BioPep00146</t>
-  </si>
-  <si>
-    <t>P01544</t>
-  </si>
-  <si>
-    <t>BioPep00147</t>
-  </si>
-  <si>
-    <t>P01545</t>
-  </si>
-  <si>
-    <t>BioPep00148</t>
-  </si>
-  <si>
-    <t>P08772</t>
-  </si>
-  <si>
-    <t>BioPep00149</t>
-  </si>
-  <si>
-    <t>P08943</t>
-  </si>
-  <si>
-    <t>BioPep00150</t>
-  </si>
-  <si>
-    <t>P09617</t>
-  </si>
-  <si>
-    <t>BioPep00151</t>
-  </si>
-  <si>
-    <t>P09618</t>
-  </si>
-  <si>
-    <t>BioPep00152</t>
-  </si>
-  <si>
-    <t>P21742</t>
-  </si>
-  <si>
-    <t>BioPep00153</t>
-  </si>
-  <si>
-    <t>P32032</t>
-  </si>
-  <si>
-    <t>BioPep00154</t>
-  </si>
-  <si>
-    <t>Q05806</t>
-  </si>
-  <si>
-    <t>BioPep00155</t>
-  </si>
-  <si>
-    <t>Q42596</t>
-  </si>
-  <si>
-    <t>BioPep00156</t>
-  </si>
-  <si>
-    <t>Q42597</t>
-  </si>
-  <si>
-    <t>BioPep00157</t>
-  </si>
-  <si>
-    <t>Q42838</t>
-  </si>
-  <si>
-    <t>BioPep00158</t>
-  </si>
-  <si>
-    <t>Q8H0Q5</t>
-  </si>
-  <si>
-    <t>BioPep00159</t>
-  </si>
-  <si>
-    <t>Q8VZK8</t>
-  </si>
-  <si>
-    <t>BioPep00160</t>
-  </si>
-  <si>
-    <t>Q9C8D6</t>
-  </si>
-  <si>
-    <t>BioPep00161</t>
-  </si>
-  <si>
-    <t>Q9SBK8</t>
-  </si>
-  <si>
-    <t>BioPep00162</t>
-  </si>
-  <si>
-    <t>P23785</t>
-  </si>
-  <si>
-    <t>BioPep00163</t>
-  </si>
-  <si>
-    <t>P28797</t>
-  </si>
-  <si>
-    <t>BioPep00164</t>
-  </si>
-  <si>
-    <t>P28798</t>
-  </si>
-  <si>
-    <t>BioPep00165</t>
-  </si>
-  <si>
-    <t>P28799</t>
-  </si>
-  <si>
-    <t>BioPep00166</t>
-  </si>
-  <si>
-    <t>Q3C258</t>
-  </si>
-  <si>
-    <t>BioPep00167</t>
-  </si>
-  <si>
-    <t>Q3C257</t>
-  </si>
-  <si>
-    <t>BioPep00168</t>
-  </si>
-  <si>
-    <t>Q3C256</t>
-  </si>
-  <si>
-    <t>BioPep00169</t>
-  </si>
-  <si>
-    <t>Q3C255</t>
-  </si>
-  <si>
-    <t>BioPep00170</t>
-  </si>
-  <si>
-    <t>A0A060QMI6</t>
-  </si>
-  <si>
-    <t>BioPep00171</t>
-  </si>
-  <si>
-    <t>Q6V1X3</t>
-  </si>
-  <si>
-    <t>BioPep00172</t>
-  </si>
-  <si>
-    <t>Q6V1X4</t>
-  </si>
-  <si>
-    <t>BioPep00173</t>
-  </si>
-  <si>
-    <t>Q6V1X5</t>
-  </si>
-  <si>
-    <t>BioPep00174</t>
-  </si>
-  <si>
-    <t>Q6V1X6</t>
-  </si>
-  <si>
-    <t>BioPep00175</t>
-  </si>
-  <si>
-    <t>Q2TM75</t>
-  </si>
-  <si>
-    <t>BioPep00176</t>
-  </si>
-  <si>
-    <t>Q6X2S3</t>
-  </si>
-  <si>
-    <t>BioPep00177</t>
-  </si>
-  <si>
-    <t>Q95KP1</t>
-  </si>
-  <si>
-    <t>BioPep00178</t>
-  </si>
-  <si>
-    <t>Q95KP2</t>
-  </si>
-  <si>
-    <t>BioPep00179</t>
-  </si>
-  <si>
-    <t>Q9DGE6</t>
-  </si>
-  <si>
-    <t>BioPep00180</t>
-  </si>
-  <si>
-    <t>Q9DGE7</t>
-  </si>
-  <si>
-    <t>BioPep00181</t>
-  </si>
-  <si>
-    <t>Q9DGE8</t>
-  </si>
-  <si>
-    <t>BioPep00182</t>
-  </si>
-  <si>
-    <t>Q9DGE9</t>
-  </si>
-  <si>
-    <t>BioPep00183</t>
-  </si>
-  <si>
-    <t>Q9DGF0</t>
-  </si>
-  <si>
-    <t>BioPep00184</t>
-  </si>
-  <si>
-    <t>Q9DGF1</t>
-  </si>
-  <si>
-    <t>BioPep00185</t>
-  </si>
-  <si>
-    <t>Q9DGF2</t>
-  </si>
-  <si>
-    <t>BioPep00186</t>
-  </si>
-  <si>
-    <t>O34163</t>
-  </si>
-  <si>
-    <t>BioPep00187</t>
-  </si>
-  <si>
-    <t>P31107</t>
-  </si>
-  <si>
-    <t>BioPep00188</t>
-  </si>
-  <si>
-    <t>C8Z3D5</t>
-  </si>
-  <si>
-    <t>BioPep00189</t>
-  </si>
-  <si>
-    <t>Q16NE8</t>
-  </si>
-  <si>
-    <t>BioPep00190</t>
-  </si>
-  <si>
-    <t>BioPep00191</t>
-  </si>
-  <si>
-    <t>P18829</t>
-  </si>
-  <si>
-    <t>BioPep00192</t>
-  </si>
-  <si>
-    <t>P18830</t>
-  </si>
-  <si>
-    <t>BioPep00193</t>
-  </si>
-  <si>
-    <t>P55319</t>
-  </si>
-  <si>
-    <t>BioPep00194</t>
-  </si>
-  <si>
-    <t>BioPep00195</t>
-  </si>
-  <si>
-    <t>C8Z3D4</t>
-  </si>
-  <si>
-    <t>BioPep00196</t>
-  </si>
-  <si>
-    <t>C8Z3D9</t>
-  </si>
-  <si>
-    <t>BioPep00197</t>
-  </si>
-  <si>
-    <t>BioPep00198</t>
-  </si>
-  <si>
-    <t>BioPep00199</t>
-  </si>
-  <si>
-    <t>P08379</t>
-  </si>
-  <si>
-    <t>BioPep00200</t>
-  </si>
-  <si>
-    <t>P35807</t>
-  </si>
-  <si>
-    <t>BioPep00201</t>
-  </si>
-  <si>
-    <t>P35808</t>
-  </si>
-  <si>
-    <t>BioPep00202</t>
-  </si>
-  <si>
-    <t>P19872</t>
-  </si>
-  <si>
-    <t>BioPep00203</t>
-  </si>
-  <si>
-    <t>P67785</t>
-  </si>
-  <si>
-    <t>BioPep00204</t>
-  </si>
-  <si>
-    <t>BioPep00205</t>
-  </si>
-  <si>
-    <t>A0ZWH7</t>
-  </si>
-  <si>
-    <t>BioPep00206</t>
-  </si>
-  <si>
-    <t>BioPep00207</t>
-  </si>
-  <si>
-    <t>BioPep00208</t>
-  </si>
-  <si>
-    <t>BioPep00209</t>
-  </si>
-  <si>
-    <t>BioPep00210</t>
-  </si>
-  <si>
-    <t>BioPep00211</t>
-  </si>
-  <si>
-    <t>BioPep00212</t>
-  </si>
-  <si>
-    <t>BioPep00213</t>
-  </si>
-  <si>
-    <t>BioPep00214</t>
-  </si>
-  <si>
-    <t>B0M2U5</t>
-  </si>
-  <si>
-    <t>BioPep00215</t>
-  </si>
-  <si>
-    <t>B0M3C0</t>
-  </si>
-  <si>
-    <t>BioPep00216</t>
-  </si>
-  <si>
-    <t>B0M3E1</t>
-  </si>
-  <si>
-    <t>BioPep00217</t>
-  </si>
-  <si>
-    <t>B3A056</t>
-  </si>
-  <si>
-    <t>BioPep00218</t>
-  </si>
-  <si>
-    <t>B3A075</t>
-  </si>
-  <si>
-    <t>BioPep00219</t>
-  </si>
-  <si>
-    <t>B3A094</t>
-  </si>
-  <si>
-    <t>BioPep00220</t>
-  </si>
-  <si>
-    <t>B3A0B4</t>
-  </si>
-  <si>
-    <t>BioPep00221</t>
-  </si>
-  <si>
-    <t>B3A0D3</t>
-  </si>
-  <si>
-    <t>BioPep00222</t>
-  </si>
-  <si>
-    <t>B3A0F2</t>
-  </si>
-  <si>
-    <t>BioPep00223</t>
-  </si>
-  <si>
-    <t>B3A0H0</t>
-  </si>
-  <si>
-    <t>BioPep00224</t>
-  </si>
-  <si>
-    <t>B3A0J0</t>
-  </si>
-  <si>
-    <t>BioPep00225</t>
-  </si>
-  <si>
-    <t>B3A0K9</t>
-  </si>
-  <si>
-    <t>BioPep00226</t>
-  </si>
-  <si>
-    <t>B3EWM7</t>
-  </si>
-  <si>
-    <t>BioPep00227</t>
-  </si>
-  <si>
-    <t>D8KXX1</t>
-  </si>
-  <si>
-    <t>BioPep00228</t>
-  </si>
-  <si>
-    <t>P14595</t>
-  </si>
-  <si>
-    <t>BioPep00229</t>
-  </si>
-  <si>
-    <t>P25418</t>
-  </si>
-  <si>
-    <t>BioPep00230</t>
-  </si>
-  <si>
-    <t>P61855</t>
-  </si>
-  <si>
-    <t>BioPep00231</t>
-  </si>
-  <si>
-    <t>P61856</t>
-  </si>
-  <si>
-    <t>BioPep00232</t>
-  </si>
-  <si>
-    <t>P67786</t>
-  </si>
-  <si>
-    <t>BioPep00233</t>
-  </si>
-  <si>
-    <t>P67787</t>
-  </si>
-  <si>
-    <t>BioPep00234</t>
-  </si>
-  <si>
-    <t>P67788</t>
-  </si>
-  <si>
-    <t>BioPep00235</t>
-  </si>
-  <si>
-    <t>P84240</t>
-  </si>
-  <si>
-    <t>BioPep00236</t>
-  </si>
-  <si>
-    <t>P84241</t>
-  </si>
-  <si>
-    <t>BioPep00237</t>
-  </si>
-  <si>
-    <t>P84242</t>
-  </si>
-  <si>
-    <t>BioPep00238</t>
-  </si>
-  <si>
-    <t>Q5EY02</t>
-  </si>
-  <si>
-    <t>BioPep00239</t>
-  </si>
-  <si>
-    <t>F8R0Y2</t>
-  </si>
-  <si>
-    <t>BioPep00240</t>
-  </si>
-  <si>
-    <t>BioPep00241</t>
-  </si>
-  <si>
-    <t>BioPep00242</t>
-  </si>
-  <si>
-    <t>BioPep00243</t>
-  </si>
-  <si>
-    <t>BioPep00244</t>
-  </si>
-  <si>
-    <t>BioPep00245</t>
-  </si>
-  <si>
-    <t>BioPep00246</t>
-  </si>
-  <si>
-    <t>BioPep00247</t>
-  </si>
-  <si>
-    <t>BioPep00248</t>
-  </si>
-  <si>
-    <t>Q5T7M4</t>
-  </si>
-  <si>
-    <t>BioPep00249</t>
-  </si>
-  <si>
-    <t>Q8R2Z0</t>
-  </si>
-  <si>
-    <t>BioPep00250</t>
-  </si>
-  <si>
-    <t>BioPep00251</t>
-  </si>
-  <si>
-    <t>BioPep00252</t>
-  </si>
-  <si>
-    <t>A1A5X5</t>
-  </si>
-  <si>
-    <t>BioPep00253</t>
-  </si>
-  <si>
-    <t>A4IH36</t>
-  </si>
-  <si>
-    <t>BioPep00254</t>
-  </si>
-  <si>
-    <t>P75409</t>
-  </si>
-  <si>
-    <t>BioPep00255</t>
-  </si>
-  <si>
-    <t>Q93Q17</t>
-  </si>
-  <si>
-    <t>BioPep00256</t>
-  </si>
-  <si>
-    <t>O62827</t>
-  </si>
-  <si>
-    <t>BioPep00257</t>
-  </si>
-  <si>
-    <t>O77559</t>
-  </si>
-  <si>
-    <t>BioPep00258</t>
-  </si>
-  <si>
-    <t>P35318</t>
-  </si>
-  <si>
-    <t>BioPep00259</t>
-  </si>
-  <si>
-    <t>P43145</t>
-  </si>
-  <si>
-    <t>BioPep00260</t>
-  </si>
-  <si>
-    <t>P53366</t>
-  </si>
-  <si>
-    <t>BioPep00261</t>
-  </si>
-  <si>
-    <t>P97297</t>
-  </si>
-  <si>
-    <t>BioPep00262</t>
-  </si>
-  <si>
-    <t>BioPep00263</t>
-  </si>
-  <si>
-    <t>P61312</t>
-  </si>
-  <si>
-    <t>BioPep00264</t>
-  </si>
-  <si>
-    <t>Q7TNK8</t>
-  </si>
-  <si>
-    <t>BioPep00265</t>
-  </si>
-  <si>
-    <t>Q7Z4H4</t>
-  </si>
-  <si>
-    <t>BioPep00266</t>
-  </si>
-  <si>
-    <t>A5LHG2</t>
-  </si>
-  <si>
-    <t>BioPep00267</t>
-  </si>
-  <si>
-    <t>P09166</t>
-  </si>
-  <si>
-    <t>BioPep00268</t>
-  </si>
-  <si>
-    <t>P09167</t>
-  </si>
-  <si>
-    <t>BioPep00269</t>
-  </si>
-  <si>
-    <t>Q06304</t>
-  </si>
-  <si>
-    <t>BioPep00270</t>
-  </si>
-  <si>
-    <t>Q08676</t>
-  </si>
-  <si>
-    <t>BioPep00271</t>
-  </si>
-  <si>
-    <t>Q06305</t>
-  </si>
-  <si>
-    <t>BioPep00272</t>
-  </si>
-  <si>
-    <t>Q06303</t>
-  </si>
-  <si>
-    <t>BioPep00273</t>
-  </si>
-  <si>
-    <t>Q06306</t>
-  </si>
-  <si>
-    <t>BioPep00274</t>
-  </si>
-  <si>
-    <t>P24856</t>
-  </si>
-  <si>
-    <t>BioPep00275</t>
-  </si>
-  <si>
-    <t>BioPep00276</t>
-  </si>
-  <si>
-    <t>BioPep00277</t>
-  </si>
-  <si>
-    <t>BioPep00278</t>
-  </si>
-  <si>
-    <t>BioPep00279</t>
-  </si>
-  <si>
-    <t>BioPep00280</t>
-  </si>
-  <si>
-    <t>BioPep00281</t>
-  </si>
-  <si>
-    <t>BioPep00282</t>
-  </si>
-  <si>
-    <t>O61466</t>
-  </si>
-  <si>
-    <t>BioPep00283</t>
-  </si>
-  <si>
-    <t>P69436</t>
-  </si>
-  <si>
-    <t>BioPep00284</t>
-  </si>
-  <si>
-    <t>P84797</t>
-  </si>
-  <si>
-    <t>BioPep00285</t>
-  </si>
-  <si>
-    <t>BioPep00286</t>
-  </si>
-  <si>
-    <t>BioPep00287</t>
-  </si>
-  <si>
-    <t>BioPep00288</t>
-  </si>
-  <si>
-    <t>BioPep00289</t>
-  </si>
-  <si>
-    <t>BioPep00290</t>
-  </si>
-  <si>
-    <t>P62926</t>
-  </si>
-  <si>
-    <t>BioPep00291</t>
-  </si>
-  <si>
-    <t>BioPep00292</t>
-  </si>
-  <si>
-    <t>P62927</t>
-  </si>
-  <si>
-    <t>BioPep00293</t>
-  </si>
-  <si>
-    <t>BioPep00294</t>
-  </si>
-  <si>
-    <t>P62928</t>
-  </si>
-  <si>
-    <t>BioPep00295</t>
-  </si>
-  <si>
-    <t>BioPep00296</t>
-  </si>
-  <si>
     <t>Q39837</t>
   </si>
   <si>
-    <t>BioPep00297</t>
-  </si>
-  <si>
-    <t>Q96474</t>
-  </si>
-  <si>
-    <t>BioPep00298</t>
-  </si>
-  <si>
-    <t>Q9FRT8</t>
-  </si>
-  <si>
-    <t>BioPep00299</t>
-  </si>
-  <si>
-    <t>Q9FRT9</t>
-  </si>
-  <si>
-    <t>BioPep00300</t>
-  </si>
-  <si>
-    <t>Q9ZQX0</t>
+    <t>BioPep00301</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +397,7 @@
   <dimension ref="A1:D9119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B252"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1739,2011 +422,1011 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A55" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A57" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A58" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A59" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A60" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A63" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A64" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A65" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A66" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A67" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A68" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A70" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A72" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A73" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A74" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A75" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A77" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A79" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A80" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A81" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A82" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A83" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A84" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A85" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A86" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A87" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A88" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A89" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A91" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>163</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A93" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A94" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A95" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A96" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A97" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A98" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A99" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A100" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A101" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>181</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A102" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>183</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A103" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>185</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A104" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>187</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A105" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A106" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A107" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A108" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>195</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A109" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A110" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A111" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A112" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A113" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A114" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A115" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A116" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A117" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A118" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A119" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A120" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>219</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A121" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A122" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A123" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>225</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A124" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A125" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>229</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A126" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A127" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A128" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A129" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>237</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A130" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A131" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>241</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A132" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A133" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A134" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A135" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A136" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>251</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A137" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>253</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A138" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>255</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A139" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>257</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A140" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A141" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A142" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A143" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A144" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>266</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A145" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A146" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A147" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>271</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A148" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A149" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>271</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A150" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A151" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A152" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>279</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A153" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A154" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A155" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>285</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A156" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A157" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>288</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A158" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>288</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A159" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A160" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>266</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A161" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A162" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A163" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>279</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A164" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A165" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A166" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>298</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A167" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>300</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A168" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A169" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>304</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A170" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>306</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A171" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>308</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A172" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>310</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A173" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>312</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A174" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>314</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A175" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>316</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A176" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>318</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A177" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>320</v>
-      </c>
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A178" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A179" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A180" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>326</v>
-      </c>
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A181" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A182" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>330</v>
-      </c>
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A183" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>332</v>
-      </c>
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A184" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>334</v>
-      </c>
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A185" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>336</v>
-      </c>
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A186" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>338</v>
-      </c>
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A187" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>340</v>
-      </c>
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A188" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>342</v>
-      </c>
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A189" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>344</v>
-      </c>
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A190" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>346</v>
-      </c>
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A191" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>348</v>
-      </c>
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A192" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A193" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>266</v>
-      </c>
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A194" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A195" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A196" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>279</v>
-      </c>
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A197" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A198" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A199" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>338</v>
-      </c>
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A200" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>358</v>
-      </c>
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A201" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>360</v>
-      </c>
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A202" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>358</v>
-      </c>
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A203" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>360</v>
-      </c>
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A204" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>364</v>
-      </c>
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A205" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>366</v>
-      </c>
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A206" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>368</v>
-      </c>
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A207" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>370</v>
-      </c>
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A208" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>372</v>
-      </c>
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A209" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>374</v>
-      </c>
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A210" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>376</v>
-      </c>
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A211" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>378</v>
-      </c>
+      <c r="A211" s="1"/>
+      <c r="B211" s="1"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A212" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>380</v>
-      </c>
+      <c r="A212" s="1"/>
+      <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A213" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>382</v>
-      </c>
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A214" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>372</v>
-      </c>
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A215" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>385</v>
-      </c>
+      <c r="A215" s="1"/>
+      <c r="B215" s="1"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A216" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>387</v>
-      </c>
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A217" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>389</v>
-      </c>
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A218" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>391</v>
-      </c>
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A219" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>393</v>
-      </c>
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A220" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>395</v>
-      </c>
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A221" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>397</v>
-      </c>
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A222" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>399</v>
-      </c>
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A223" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>401</v>
-      </c>
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A224" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>403</v>
-      </c>
+      <c r="A224" s="1"/>
+      <c r="B224" s="1"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A225" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>405</v>
-      </c>
+      <c r="A225" s="1"/>
+      <c r="B225" s="1"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A226" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A227" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A227" s="1"/>
+      <c r="B227" s="1"/>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A228" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A228" s="1"/>
+      <c r="B228" s="1"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A229" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A230" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A231" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A231" s="1"/>
+      <c r="B231" s="1"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A232" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A232" s="1"/>
+      <c r="B232" s="1"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A233" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A234" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>416</v>
-      </c>
+      <c r="A234" s="1"/>
+      <c r="B234" s="1"/>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A235" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>418</v>
-      </c>
+      <c r="A235" s="1"/>
+      <c r="B235" s="1"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A236" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>420</v>
-      </c>
+      <c r="A236" s="1"/>
+      <c r="B236" s="1"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A237" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A237" s="1"/>
+      <c r="B237" s="1"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A238" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>271</v>
-      </c>
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A239" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A240" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A241" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A242" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>427</v>
-      </c>
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A243" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>427</v>
-      </c>
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A244" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A245" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A246" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>433</v>
-      </c>
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A247" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>433</v>
-      </c>
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A248" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>436</v>
-      </c>
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A249" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>438</v>
-      </c>
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A250" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>440</v>
-      </c>
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A251" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>442</v>
-      </c>
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A252" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>444</v>
-      </c>
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A253" s="1"/>
@@ -3998,264 +1681,264 @@
       <c r="B315" s="1"/>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A316" s="2"/>
-      <c r="B316" s="2"/>
+      <c r="A316" s="1"/>
+      <c r="B316" s="1"/>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A317" s="2"/>
-      <c r="B317" s="2"/>
+      <c r="A317" s="1"/>
+      <c r="B317" s="1"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A318" s="2"/>
-      <c r="B318" s="2"/>
+      <c r="A318" s="1"/>
+      <c r="B318" s="1"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A319" s="2"/>
-      <c r="B319" s="2"/>
+      <c r="A319" s="1"/>
+      <c r="B319" s="1"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A320" s="2"/>
-      <c r="B320" s="2"/>
+      <c r="A320" s="1"/>
+      <c r="B320" s="1"/>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A321" s="2"/>
-      <c r="B321" s="2"/>
+      <c r="A321" s="1"/>
+      <c r="B321" s="1"/>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A322" s="2"/>
-      <c r="B322" s="2"/>
+      <c r="A322" s="1"/>
+      <c r="B322" s="1"/>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A323" s="2"/>
-      <c r="B323" s="2"/>
+      <c r="A323" s="1"/>
+      <c r="B323" s="1"/>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A324" s="2"/>
-      <c r="B324" s="2"/>
+      <c r="A324" s="1"/>
+      <c r="B324" s="1"/>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A325" s="2"/>
-      <c r="B325" s="2"/>
+      <c r="A325" s="1"/>
+      <c r="B325" s="1"/>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A326" s="2"/>
-      <c r="B326" s="2"/>
+      <c r="A326" s="1"/>
+      <c r="B326" s="1"/>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A327" s="2"/>
-      <c r="B327" s="2"/>
+      <c r="A327" s="1"/>
+      <c r="B327" s="1"/>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A328" s="2"/>
-      <c r="B328" s="2"/>
+      <c r="A328" s="1"/>
+      <c r="B328" s="1"/>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A329" s="2"/>
-      <c r="B329" s="2"/>
+      <c r="A329" s="1"/>
+      <c r="B329" s="1"/>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A330" s="2"/>
-      <c r="B330" s="2"/>
+      <c r="A330" s="1"/>
+      <c r="B330" s="1"/>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A331" s="2"/>
-      <c r="B331" s="2"/>
+      <c r="A331" s="1"/>
+      <c r="B331" s="1"/>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A332" s="2"/>
-      <c r="B332" s="2"/>
+      <c r="A332" s="1"/>
+      <c r="B332" s="1"/>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A333" s="2"/>
-      <c r="B333" s="2"/>
+      <c r="A333" s="1"/>
+      <c r="B333" s="1"/>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A334" s="2"/>
-      <c r="B334" s="2"/>
+      <c r="A334" s="1"/>
+      <c r="B334" s="1"/>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A335" s="2"/>
-      <c r="B335" s="2"/>
+      <c r="A335" s="1"/>
+      <c r="B335" s="1"/>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A336" s="2"/>
-      <c r="B336" s="2"/>
+      <c r="A336" s="1"/>
+      <c r="B336" s="1"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A337" s="2"/>
-      <c r="B337" s="2"/>
+      <c r="A337" s="1"/>
+      <c r="B337" s="1"/>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A338" s="2"/>
-      <c r="B338" s="2"/>
+      <c r="A338" s="1"/>
+      <c r="B338" s="1"/>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A339" s="2"/>
-      <c r="B339" s="2"/>
+      <c r="A339" s="1"/>
+      <c r="B339" s="1"/>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A340" s="2"/>
-      <c r="B340" s="2"/>
+      <c r="A340" s="1"/>
+      <c r="B340" s="1"/>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A341" s="2"/>
-      <c r="B341" s="2"/>
+      <c r="A341" s="1"/>
+      <c r="B341" s="1"/>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A342" s="2"/>
-      <c r="B342" s="2"/>
+      <c r="A342" s="1"/>
+      <c r="B342" s="1"/>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A343" s="2"/>
-      <c r="B343" s="2"/>
+      <c r="A343" s="1"/>
+      <c r="B343" s="1"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A344" s="2"/>
-      <c r="B344" s="2"/>
+      <c r="A344" s="1"/>
+      <c r="B344" s="1"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A345" s="2"/>
-      <c r="B345" s="2"/>
+      <c r="A345" s="1"/>
+      <c r="B345" s="1"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A346" s="2"/>
-      <c r="B346" s="2"/>
+      <c r="A346" s="1"/>
+      <c r="B346" s="1"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A347" s="2"/>
-      <c r="B347" s="2"/>
+      <c r="A347" s="1"/>
+      <c r="B347" s="1"/>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A348" s="2"/>
-      <c r="B348" s="2"/>
+      <c r="A348" s="1"/>
+      <c r="B348" s="1"/>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A349" s="2"/>
-      <c r="B349" s="2"/>
+      <c r="A349" s="1"/>
+      <c r="B349" s="1"/>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A350" s="2"/>
-      <c r="B350" s="2"/>
+      <c r="A350" s="1"/>
+      <c r="B350" s="1"/>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A351" s="2"/>
-      <c r="B351" s="2"/>
+      <c r="A351" s="1"/>
+      <c r="B351" s="1"/>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A352" s="2"/>
-      <c r="B352" s="2"/>
+      <c r="A352" s="1"/>
+      <c r="B352" s="1"/>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A353" s="2"/>
-      <c r="B353" s="2"/>
+      <c r="A353" s="1"/>
+      <c r="B353" s="1"/>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A354" s="2"/>
-      <c r="B354" s="2"/>
+      <c r="A354" s="1"/>
+      <c r="B354" s="1"/>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A355" s="2"/>
-      <c r="B355" s="2"/>
+      <c r="A355" s="1"/>
+      <c r="B355" s="1"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A356" s="2"/>
-      <c r="B356" s="2"/>
+      <c r="A356" s="1"/>
+      <c r="B356" s="1"/>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A357" s="2"/>
-      <c r="B357" s="2"/>
+      <c r="A357" s="1"/>
+      <c r="B357" s="1"/>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A358" s="2"/>
-      <c r="B358" s="2"/>
+      <c r="A358" s="1"/>
+      <c r="B358" s="1"/>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A359" s="2"/>
-      <c r="B359" s="2"/>
+      <c r="A359" s="1"/>
+      <c r="B359" s="1"/>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A360" s="2"/>
-      <c r="B360" s="2"/>
+      <c r="A360" s="1"/>
+      <c r="B360" s="1"/>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A361" s="2"/>
-      <c r="B361" s="2"/>
+      <c r="A361" s="1"/>
+      <c r="B361" s="1"/>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A362" s="2"/>
-      <c r="B362" s="2"/>
+      <c r="A362" s="1"/>
+      <c r="B362" s="1"/>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A363" s="2"/>
-      <c r="B363" s="2"/>
+      <c r="A363" s="1"/>
+      <c r="B363" s="1"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A364" s="2"/>
-      <c r="B364" s="2"/>
+      <c r="A364" s="1"/>
+      <c r="B364" s="1"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A365" s="2"/>
-      <c r="B365" s="2"/>
+      <c r="A365" s="1"/>
+      <c r="B365" s="1"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A366" s="2"/>
-      <c r="B366" s="2"/>
+      <c r="A366" s="1"/>
+      <c r="B366" s="1"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A367" s="2"/>
-      <c r="B367" s="2"/>
+      <c r="A367" s="1"/>
+      <c r="B367" s="1"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A368" s="2"/>
-      <c r="B368" s="2"/>
+      <c r="A368" s="1"/>
+      <c r="B368" s="1"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A369" s="2"/>
-      <c r="B369" s="2"/>
+      <c r="A369" s="1"/>
+      <c r="B369" s="1"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A370" s="2"/>
-      <c r="B370" s="2"/>
+      <c r="A370" s="1"/>
+      <c r="B370" s="1"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A371" s="2"/>
-      <c r="B371" s="2"/>
+      <c r="A371" s="1"/>
+      <c r="B371" s="1"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A372" s="2"/>
-      <c r="B372" s="2"/>
+      <c r="A372" s="1"/>
+      <c r="B372" s="1"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A373" s="2"/>
-      <c r="B373" s="2"/>
+      <c r="A373" s="1"/>
+      <c r="B373" s="1"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A374" s="2"/>
-      <c r="B374" s="2"/>
+      <c r="A374" s="1"/>
+      <c r="B374" s="1"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A375" s="2"/>
-      <c r="B375" s="2"/>
+      <c r="A375" s="1"/>
+      <c r="B375" s="1"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A376" s="2"/>
-      <c r="B376" s="2"/>
+      <c r="A376" s="1"/>
+      <c r="B376" s="1"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A377" s="2"/>
-      <c r="B377" s="2"/>
+      <c r="A377" s="1"/>
+      <c r="B377" s="1"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A378" s="2"/>
-      <c r="B378" s="2"/>
+      <c r="A378" s="1"/>
+      <c r="B378" s="1"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A379" s="2"/>
-      <c r="B379" s="2"/>
+      <c r="A379" s="1"/>
+      <c r="B379" s="1"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A380" s="2"/>
-      <c r="B380" s="2"/>
+      <c r="A380" s="1"/>
+      <c r="B380" s="1"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A381" s="2"/>

</xml_diff>

<commit_message>
2015.2.2 multi input option
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="340">
   <si>
     <t>ID</t>
   </si>
@@ -30,10 +30,1012 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Q39837</t>
+    <t>BioPep02311</t>
   </si>
   <si>
-    <t>BioPep00301</t>
+    <t>P0C5X3</t>
+  </si>
+  <si>
+    <t>BioPep02312</t>
+  </si>
+  <si>
+    <t>P0C5X4</t>
+  </si>
+  <si>
+    <t>BioPep02313</t>
+  </si>
+  <si>
+    <t>P0C5X5</t>
+  </si>
+  <si>
+    <t>BioPep02314</t>
+  </si>
+  <si>
+    <t>P32413</t>
+  </si>
+  <si>
+    <t>BioPep02315</t>
+  </si>
+  <si>
+    <t>P40837</t>
+  </si>
+  <si>
+    <t>BioPep02316</t>
+  </si>
+  <si>
+    <t>P40838</t>
+  </si>
+  <si>
+    <t>BioPep02317</t>
+  </si>
+  <si>
+    <t>P40839</t>
+  </si>
+  <si>
+    <t>BioPep02318</t>
+  </si>
+  <si>
+    <t>P84842</t>
+  </si>
+  <si>
+    <t>BioPep02319</t>
+  </si>
+  <si>
+    <t>P86151</t>
+  </si>
+  <si>
+    <t>BioPep02320</t>
+  </si>
+  <si>
+    <t>P40840</t>
+  </si>
+  <si>
+    <t>BioPep02321</t>
+  </si>
+  <si>
+    <t>P40841</t>
+  </si>
+  <si>
+    <t>BioPep02322</t>
+  </si>
+  <si>
+    <t>P40842</t>
+  </si>
+  <si>
+    <t>BioPep02323</t>
+  </si>
+  <si>
+    <t>P86153</t>
+  </si>
+  <si>
+    <t>BioPep02324</t>
+  </si>
+  <si>
+    <t>P86154</t>
+  </si>
+  <si>
+    <t>BioPep02325</t>
+  </si>
+  <si>
+    <t>P86152</t>
+  </si>
+  <si>
+    <t>BioPep02326</t>
+  </si>
+  <si>
+    <t>P84860</t>
+  </si>
+  <si>
+    <t>BioPep02327</t>
+  </si>
+  <si>
+    <t>A0AEI5</t>
+  </si>
+  <si>
+    <t>BioPep02328</t>
+  </si>
+  <si>
+    <t>A0AEI6</t>
+  </si>
+  <si>
+    <t>BioPep02329</t>
+  </si>
+  <si>
+    <t>B4ERK4</t>
+  </si>
+  <si>
+    <t>BioPep02330</t>
+  </si>
+  <si>
+    <t>E7EKE0</t>
+  </si>
+  <si>
+    <t>BioPep02331</t>
+  </si>
+  <si>
+    <t>E7EKE1</t>
+  </si>
+  <si>
+    <t>BioPep02332</t>
+  </si>
+  <si>
+    <t>P0C8S9</t>
+  </si>
+  <si>
+    <t>BioPep02333</t>
+  </si>
+  <si>
+    <t>P0C8T0</t>
+  </si>
+  <si>
+    <t>BioPep02334</t>
+  </si>
+  <si>
+    <t>B3A0M3</t>
+  </si>
+  <si>
+    <t>BioPep02335</t>
+  </si>
+  <si>
+    <t>G3E7P5</t>
+  </si>
+  <si>
+    <t>BioPep02336</t>
+  </si>
+  <si>
+    <t>G3E7P6</t>
+  </si>
+  <si>
+    <t>BioPep02337</t>
+  </si>
+  <si>
+    <t>G3E7P7</t>
+  </si>
+  <si>
+    <t>BioPep02338</t>
+  </si>
+  <si>
+    <t>G3E7P8</t>
+  </si>
+  <si>
+    <t>BioPep02339</t>
+  </si>
+  <si>
+    <t>G3E7P9</t>
+  </si>
+  <si>
+    <t>BioPep02340</t>
+  </si>
+  <si>
+    <t>G3E7Q0</t>
+  </si>
+  <si>
+    <t>BioPep02341</t>
+  </si>
+  <si>
+    <t>G3E7Q1</t>
+  </si>
+  <si>
+    <t>BioPep02342</t>
+  </si>
+  <si>
+    <t>P0C8T3</t>
+  </si>
+  <si>
+    <t>BioPep02343</t>
+  </si>
+  <si>
+    <t>P0C8T4</t>
+  </si>
+  <si>
+    <t>BioPep02344</t>
+  </si>
+  <si>
+    <t>P0C8T5</t>
+  </si>
+  <si>
+    <t>BioPep02345</t>
+  </si>
+  <si>
+    <t>P0C8T6</t>
+  </si>
+  <si>
+    <t>BioPep02346</t>
+  </si>
+  <si>
+    <t>P0C8T7</t>
+  </si>
+  <si>
+    <t>BioPep02347</t>
+  </si>
+  <si>
+    <t>P85095</t>
+  </si>
+  <si>
+    <t>BioPep02348</t>
+  </si>
+  <si>
+    <t>P86022</t>
+  </si>
+  <si>
+    <t>BioPep02349</t>
+  </si>
+  <si>
+    <t>P86023</t>
+  </si>
+  <si>
+    <t>BioPep02350</t>
+  </si>
+  <si>
+    <t>P86024</t>
+  </si>
+  <si>
+    <t>BioPep02351</t>
+  </si>
+  <si>
+    <t>P86025</t>
+  </si>
+  <si>
+    <t>BioPep02352</t>
+  </si>
+  <si>
+    <t>P82268</t>
+  </si>
+  <si>
+    <t>BioPep02353</t>
+  </si>
+  <si>
+    <t>P82269</t>
+  </si>
+  <si>
+    <t>BioPep02354</t>
+  </si>
+  <si>
+    <t>P82234</t>
+  </si>
+  <si>
+    <t>BioPep02355</t>
+  </si>
+  <si>
+    <t>P82235</t>
+  </si>
+  <si>
+    <t>BioPep02356</t>
+  </si>
+  <si>
+    <t>P58803</t>
+  </si>
+  <si>
+    <t>BioPep02357</t>
+  </si>
+  <si>
+    <t>P58804</t>
+  </si>
+  <si>
+    <t>BioPep02358</t>
+  </si>
+  <si>
+    <t>P83346</t>
+  </si>
+  <si>
+    <t>BioPep02359</t>
+  </si>
+  <si>
+    <t>P81782</t>
+  </si>
+  <si>
+    <t>BioPep02360</t>
+  </si>
+  <si>
+    <t>P20481</t>
+  </si>
+  <si>
+    <t>BioPep02361</t>
+  </si>
+  <si>
+    <t>BioPep02362</t>
+  </si>
+  <si>
+    <t>BioPep02363</t>
+  </si>
+  <si>
+    <t>BioPep02364</t>
+  </si>
+  <si>
+    <t>BioPep02365</t>
+  </si>
+  <si>
+    <t>BioPep02366</t>
+  </si>
+  <si>
+    <t>BioPep02367</t>
+  </si>
+  <si>
+    <t>BioPep02368</t>
+  </si>
+  <si>
+    <t>BioPep02369</t>
+  </si>
+  <si>
+    <t>BioPep02370</t>
+  </si>
+  <si>
+    <t>BioPep02371</t>
+  </si>
+  <si>
+    <t>BioPep02372</t>
+  </si>
+  <si>
+    <t>BioPep02373</t>
+  </si>
+  <si>
+    <t>BioPep02374</t>
+  </si>
+  <si>
+    <t>BioPep02375</t>
+  </si>
+  <si>
+    <t>BioPep02376</t>
+  </si>
+  <si>
+    <t>BioPep02377</t>
+  </si>
+  <si>
+    <t>BioPep02378</t>
+  </si>
+  <si>
+    <t>BioPep02379</t>
+  </si>
+  <si>
+    <t>BioPep02380</t>
+  </si>
+  <si>
+    <t>BioPep02381</t>
+  </si>
+  <si>
+    <t>C0HJB7</t>
+  </si>
+  <si>
+    <t>BioPep02382</t>
+  </si>
+  <si>
+    <t>P82815</t>
+  </si>
+  <si>
+    <t>BioPep02383</t>
+  </si>
+  <si>
+    <t>A2VB89</t>
+  </si>
+  <si>
+    <t>BioPep02384</t>
+  </si>
+  <si>
+    <t>P84118</t>
+  </si>
+  <si>
+    <t>BioPep02385</t>
+  </si>
+  <si>
+    <t>P85315</t>
+  </si>
+  <si>
+    <t>BioPep02386</t>
+  </si>
+  <si>
+    <t>P85316</t>
+  </si>
+  <si>
+    <t>BioPep02387</t>
+  </si>
+  <si>
+    <t>Q4FCM6</t>
+  </si>
+  <si>
+    <t>BioPep02388</t>
+  </si>
+  <si>
+    <t>Q566B1</t>
+  </si>
+  <si>
+    <t>BioPep02389</t>
+  </si>
+  <si>
+    <t>Q66Q82</t>
+  </si>
+  <si>
+    <t>BioPep02390</t>
+  </si>
+  <si>
+    <t>Q9VD83</t>
+  </si>
+  <si>
+    <t>BioPep02391</t>
+  </si>
+  <si>
+    <t>P56685</t>
+  </si>
+  <si>
+    <t>BioPep02392</t>
+  </si>
+  <si>
+    <t>Q6XVK6</t>
+  </si>
+  <si>
+    <t>BioPep02393</t>
+  </si>
+  <si>
+    <t>Q6XVK7</t>
+  </si>
+  <si>
+    <t>BioPep02394</t>
+  </si>
+  <si>
+    <t>Q6XVK8</t>
+  </si>
+  <si>
+    <t>BioPep02395</t>
+  </si>
+  <si>
+    <t>Q6XVK9</t>
+  </si>
+  <si>
+    <t>BioPep02396</t>
+  </si>
+  <si>
+    <t>Q6XVL1</t>
+  </si>
+  <si>
+    <t>BioPep02397</t>
+  </si>
+  <si>
+    <t>Q6XVL2</t>
+  </si>
+  <si>
+    <t>BioPep02398</t>
+  </si>
+  <si>
+    <t>Q6XVL3</t>
+  </si>
+  <si>
+    <t>BioPep02399</t>
+  </si>
+  <si>
+    <t>Q6XVL4</t>
+  </si>
+  <si>
+    <t>BioPep02400</t>
+  </si>
+  <si>
+    <t>Q6XVL5</t>
+  </si>
+  <si>
+    <t>BioPep02401</t>
+  </si>
+  <si>
+    <t>Q6XVL7</t>
+  </si>
+  <si>
+    <t>BioPep02402</t>
+  </si>
+  <si>
+    <t>Q6XVL8</t>
+  </si>
+  <si>
+    <t>BioPep02403</t>
+  </si>
+  <si>
+    <t>Q6XVM1</t>
+  </si>
+  <si>
+    <t>BioPep02404</t>
+  </si>
+  <si>
+    <t>Q6XVM2</t>
+  </si>
+  <si>
+    <t>BioPep02405</t>
+  </si>
+  <si>
+    <t>Q6XVM4</t>
+  </si>
+  <si>
+    <t>BioPep02406</t>
+  </si>
+  <si>
+    <t>Q6XVM6</t>
+  </si>
+  <si>
+    <t>BioPep02407</t>
+  </si>
+  <si>
+    <t>Q6XVM7</t>
+  </si>
+  <si>
+    <t>BioPep02408</t>
+  </si>
+  <si>
+    <t>Q6XVM8</t>
+  </si>
+  <si>
+    <t>BioPep02409</t>
+  </si>
+  <si>
+    <t>Q6XVM9</t>
+  </si>
+  <si>
+    <t>BioPep02410</t>
+  </si>
+  <si>
+    <t>Q6XVN0</t>
+  </si>
+  <si>
+    <t>BioPep02411</t>
+  </si>
+  <si>
+    <t>Q6XVN2</t>
+  </si>
+  <si>
+    <t>BioPep02412</t>
+  </si>
+  <si>
+    <t>Q6XVN3</t>
+  </si>
+  <si>
+    <t>BioPep02413</t>
+  </si>
+  <si>
+    <t>P62564</t>
+  </si>
+  <si>
+    <t>BioPep02414</t>
+  </si>
+  <si>
+    <t>P62565</t>
+  </si>
+  <si>
+    <t>BioPep02415</t>
+  </si>
+  <si>
+    <t>P62566</t>
+  </si>
+  <si>
+    <t>BioPep02416</t>
+  </si>
+  <si>
+    <t>P62567</t>
+  </si>
+  <si>
+    <t>BioPep02417</t>
+  </si>
+  <si>
+    <t>P62581</t>
+  </si>
+  <si>
+    <t>BioPep02418</t>
+  </si>
+  <si>
+    <t>P62582</t>
+  </si>
+  <si>
+    <t>BioPep02419</t>
+  </si>
+  <si>
+    <t>P56247</t>
+  </si>
+  <si>
+    <t>BioPep02420</t>
+  </si>
+  <si>
+    <t>P56248</t>
+  </si>
+  <si>
+    <t>BioPep02421</t>
+  </si>
+  <si>
+    <t>P82076</t>
+  </si>
+  <si>
+    <t>BioPep02422</t>
+  </si>
+  <si>
+    <t>P82077</t>
+  </si>
+  <si>
+    <t>BioPep02423</t>
+  </si>
+  <si>
+    <t>P82078</t>
+  </si>
+  <si>
+    <t>BioPep02424</t>
+  </si>
+  <si>
+    <t>P82051</t>
+  </si>
+  <si>
+    <t>BioPep02425</t>
+  </si>
+  <si>
+    <t>B5AKW4</t>
+  </si>
+  <si>
+    <t>BioPep02426</t>
+  </si>
+  <si>
+    <t>B5AKW5</t>
+  </si>
+  <si>
+    <t>BioPep02427</t>
+  </si>
+  <si>
+    <t>P86484</t>
+  </si>
+  <si>
+    <t>BioPep02428</t>
+  </si>
+  <si>
+    <t>P86485</t>
+  </si>
+  <si>
+    <t>BioPep02429</t>
+  </si>
+  <si>
+    <t>P62568</t>
+  </si>
+  <si>
+    <t>BioPep02430</t>
+  </si>
+  <si>
+    <t>P62569</t>
+  </si>
+  <si>
+    <t>BioPep02431</t>
+  </si>
+  <si>
+    <t>P86501</t>
+  </si>
+  <si>
+    <t>BioPep02432</t>
+  </si>
+  <si>
+    <t>Q800R2</t>
+  </si>
+  <si>
+    <t>BioPep02433</t>
+  </si>
+  <si>
+    <t>BioPep02434</t>
+  </si>
+  <si>
+    <t>BioPep02435</t>
+  </si>
+  <si>
+    <t>BioPep02436</t>
+  </si>
+  <si>
+    <t>BioPep02437</t>
+  </si>
+  <si>
+    <t>BioPep02438</t>
+  </si>
+  <si>
+    <t>BioPep02439</t>
+  </si>
+  <si>
+    <t>BioPep02440</t>
+  </si>
+  <si>
+    <t>BioPep02441</t>
+  </si>
+  <si>
+    <t>BioPep02442</t>
+  </si>
+  <si>
+    <t>BioPep02443</t>
+  </si>
+  <si>
+    <t>BioPep02444</t>
+  </si>
+  <si>
+    <t>P82104</t>
+  </si>
+  <si>
+    <t>BioPep02445</t>
+  </si>
+  <si>
+    <t>P86502</t>
+  </si>
+  <si>
+    <t>BioPep02446</t>
+  </si>
+  <si>
+    <t>P86503</t>
+  </si>
+  <si>
+    <t>BioPep02447</t>
+  </si>
+  <si>
+    <t>P0C2A6</t>
+  </si>
+  <si>
+    <t>BioPep02448</t>
+  </si>
+  <si>
+    <t>BioPep02449</t>
+  </si>
+  <si>
+    <t>BioPep02450</t>
+  </si>
+  <si>
+    <t>P0C2A7</t>
+  </si>
+  <si>
+    <t>BioPep02451</t>
+  </si>
+  <si>
+    <t>P0C2A8</t>
+  </si>
+  <si>
+    <t>BioPep02452</t>
+  </si>
+  <si>
+    <t>BioPep02453</t>
+  </si>
+  <si>
+    <t>BioPep02454</t>
+  </si>
+  <si>
+    <t>BioPep02455</t>
+  </si>
+  <si>
+    <t>P56227</t>
+  </si>
+  <si>
+    <t>BioPep02456</t>
+  </si>
+  <si>
+    <t>P56228</t>
+  </si>
+  <si>
+    <t>BioPep02457</t>
+  </si>
+  <si>
+    <t>P62544</t>
+  </si>
+  <si>
+    <t>BioPep02458</t>
+  </si>
+  <si>
+    <t>P62545</t>
+  </si>
+  <si>
+    <t>BioPep02459</t>
+  </si>
+  <si>
+    <t>BioPep02460</t>
+  </si>
+  <si>
+    <t>BioPep02461</t>
+  </si>
+  <si>
+    <t>P56230</t>
+  </si>
+  <si>
+    <t>BioPep02462</t>
+  </si>
+  <si>
+    <t>P62546</t>
+  </si>
+  <si>
+    <t>BioPep02463</t>
+  </si>
+  <si>
+    <t>P62547</t>
+  </si>
+  <si>
+    <t>BioPep02464</t>
+  </si>
+  <si>
+    <t>BioPep02465</t>
+  </si>
+  <si>
+    <t>BioPep02466</t>
+  </si>
+  <si>
+    <t>P62548</t>
+  </si>
+  <si>
+    <t>BioPep02467</t>
+  </si>
+  <si>
+    <t>P62549</t>
+  </si>
+  <si>
+    <t>BioPep02468</t>
+  </si>
+  <si>
+    <t>BioPep02469</t>
+  </si>
+  <si>
+    <t>BioPep02470</t>
+  </si>
+  <si>
+    <t>P81251</t>
+  </si>
+  <si>
+    <t>BioPep02471</t>
+  </si>
+  <si>
+    <t>P81252</t>
+  </si>
+  <si>
+    <t>BioPep02472</t>
+  </si>
+  <si>
+    <t>P56233</t>
+  </si>
+  <si>
+    <t>BioPep02473</t>
+  </si>
+  <si>
+    <t>P86504</t>
+  </si>
+  <si>
+    <t>BioPep02474</t>
+  </si>
+  <si>
+    <t>P62570</t>
+  </si>
+  <si>
+    <t>BioPep02475</t>
+  </si>
+  <si>
+    <t>P62571</t>
+  </si>
+  <si>
+    <t>BioPep02476</t>
+  </si>
+  <si>
+    <t>BioPep02477</t>
+  </si>
+  <si>
+    <t>BioPep02478</t>
+  </si>
+  <si>
+    <t>P69032</t>
+  </si>
+  <si>
+    <t>BioPep02479</t>
+  </si>
+  <si>
+    <t>P56236</t>
+  </si>
+  <si>
+    <t>BioPep02480</t>
+  </si>
+  <si>
+    <t>P56237</t>
+  </si>
+  <si>
+    <t>BioPep02481</t>
+  </si>
+  <si>
+    <t>P62562</t>
+  </si>
+  <si>
+    <t>BioPep02482</t>
+  </si>
+  <si>
+    <t>P62563</t>
+  </si>
+  <si>
+    <t>BioPep02483</t>
+  </si>
+  <si>
+    <t>P86505</t>
+  </si>
+  <si>
+    <t>BioPep02484</t>
+  </si>
+  <si>
+    <t>P56239</t>
+  </si>
+  <si>
+    <t>BioPep02485</t>
+  </si>
+  <si>
+    <t>P56240</t>
+  </si>
+  <si>
+    <t>BioPep02486</t>
+  </si>
+  <si>
+    <t>P56241</t>
+  </si>
+  <si>
+    <t>BioPep02487</t>
+  </si>
+  <si>
+    <t>P0C2A9</t>
+  </si>
+  <si>
+    <t>BioPep02488</t>
+  </si>
+  <si>
+    <t>P56242</t>
+  </si>
+  <si>
+    <t>BioPep02489</t>
+  </si>
+  <si>
+    <t>P56243</t>
+  </si>
+  <si>
+    <t>BioPep02490</t>
+  </si>
+  <si>
+    <t>P56244</t>
+  </si>
+  <si>
+    <t>BioPep02491</t>
+  </si>
+  <si>
+    <t>P86506</t>
+  </si>
+  <si>
+    <t>BioPep02492</t>
+  </si>
+  <si>
+    <t>P86507</t>
+  </si>
+  <si>
+    <t>BioPep02493</t>
+  </si>
+  <si>
+    <t>P01357</t>
+  </si>
+  <si>
+    <t>BioPep02494</t>
+  </si>
+  <si>
+    <t>P05222</t>
+  </si>
+  <si>
+    <t>BioPep02495</t>
+  </si>
+  <si>
+    <t>P05224</t>
+  </si>
+  <si>
+    <t>BioPep02496</t>
+  </si>
+  <si>
+    <t>P05225</t>
+  </si>
+  <si>
+    <t>BioPep02497</t>
+  </si>
+  <si>
+    <t>P05226</t>
+  </si>
+  <si>
+    <t>BioPep02498</t>
+  </si>
+  <si>
+    <t>P56264</t>
+  </si>
+  <si>
+    <t>BioPep02499</t>
+  </si>
+  <si>
+    <t>P86486</t>
+  </si>
+  <si>
+    <t>BioPep02500</t>
+  </si>
+  <si>
+    <t>P62541</t>
   </si>
 </sst>
 </file>
@@ -397,7 +1399,7 @@
   <dimension ref="A1:D9119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -422,767 +1424,1523 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="A67" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
+      <c r="A82" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+      <c r="A84" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
+      <c r="A85" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
+      <c r="A86" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
+      <c r="A88" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
+      <c r="A89" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+      <c r="A90" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+      <c r="A92" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
+      <c r="A93" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+      <c r="A94" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
+      <c r="A97" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
+      <c r="A98" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
+      <c r="A100" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
+      <c r="A101" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
+      <c r="A104" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
+      <c r="A105" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
+      <c r="A106" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
+      <c r="A108" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
+      <c r="A114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
+      <c r="A115" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
+      <c r="A116" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
+      <c r="A117" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+      <c r="A120" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
+      <c r="A125" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
+      <c r="A127" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
+      <c r="A129" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
+      <c r="A130" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
+      <c r="A131" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
+      <c r="A133" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
+      <c r="A134" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
+      <c r="A135" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
+      <c r="A136" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
+      <c r="A137" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+      <c r="A138" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
+      <c r="A139" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
+      <c r="A140" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
+      <c r="A141" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
+      <c r="A144" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
+      <c r="A145" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
+      <c r="A146" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
+      <c r="A147" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
+      <c r="A148" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
+      <c r="A149" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
+      <c r="A150" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
+      <c r="A152" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
+      <c r="A153" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
+      <c r="A156" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
+      <c r="A160" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
+      <c r="A161" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
+      <c r="A162" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
+      <c r="A164" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
+      <c r="A165" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
+      <c r="A166" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
+      <c r="A168" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
+      <c r="A169" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
+      <c r="A170" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
+      <c r="A171" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
+      <c r="A173" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
+      <c r="A174" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
+      <c r="A175" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
+      <c r="A176" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
+      <c r="A177" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
+      <c r="A178" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
+      <c r="A179" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
+      <c r="A180" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
+      <c r="A182" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
+      <c r="A183" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
+      <c r="A184" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
+      <c r="A185" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
+      <c r="A186" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
+      <c r="A187" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
+      <c r="A188" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
+      <c r="A189" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
+      <c r="A190" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
+      <c r="A191" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A192" s="1"/>

</xml_diff>